<commit_message>
updating the unsupervised ML notebook and other changes
</commit_message>
<xml_diff>
--- a/ramandecompy/tests/test_files/CalibrationSpectraCombined.xlsx
+++ b/ramandecompy/tests/test_files/CalibrationSpectraCombined.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elizabeth/Desktop/raman-spectra-decomp-analysis/ramandecompy/tests/test_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{48D5E89E-C165-5C44-BC78-0B5B73A04F93}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B92C01E0-EAC0-EF43-847B-B415C7A1AC03}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="13980" windowHeight="17040" xr2:uid="{D22CC806-908B-EB49-9294-8AC28401A05D}"/>
+    <workbookView xWindow="1420" yWindow="460" windowWidth="13980" windowHeight="17040" xr2:uid="{D22CC806-908B-EB49-9294-8AC28401A05D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -57,13 +57,13 @@
     <t>Ethane</t>
   </si>
   <si>
-    <t>Formic Acid</t>
-  </si>
-  <si>
     <t>Methane</t>
   </si>
   <si>
     <t>Propane</t>
+  </si>
+  <si>
+    <t>FormicAcid</t>
   </si>
 </sst>
 </file>
@@ -418,7 +418,7 @@
   <dimension ref="A1:K1942"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -444,7 +444,7 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="G1" t="s">
         <v>5</v>
@@ -456,10 +456,10 @@
         <v>7</v>
       </c>
       <c r="J1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" t="s">
         <v>9</v>
-      </c>
-      <c r="K1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">

</xml_diff>